<commit_message>
FMKIO CodeGen config done
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbarb\Documents\PlatformIO\Projects\STM32_tplprj\Doc\ConfigPrj\ExcelCfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAD6D6B-382C-4BA7-92BD-418C94B4041A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9566025B-F27D-4E4F-A6B6-3F68DA963F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="C18:V43"/>
   <sheetViews>
-    <sheetView topLeftCell="E14" zoomScale="89" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="E14" zoomScale="89" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="M19">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O19" t="s">
         <v>17</v>
@@ -1095,7 +1095,7 @@
         <v>13</v>
       </c>
       <c r="M20">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.3">
@@ -1118,7 +1118,7 @@
         <v>14</v>
       </c>
       <c r="M21">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.3">
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
   <dimension ref="A4:AF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="I1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Code gen for module FMKCPU done
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbarb\Documents\PlatformIO\Projects\STM32_tplprj\Doc\ConfigPrj\ExcelCfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9566025B-F27D-4E4F-A6B6-3F68DA963F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808D4FDA-0D0B-4C18-852F-36942223AFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="151">
   <si>
     <t>Colonne1</t>
   </si>
@@ -119,75 +119,6 @@
     <t>RCC_ClockName</t>
   </si>
   <si>
-    <t>FMKCPU_RCC_CLK_SYSCFG</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_ADC1</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_TIM1</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_TIM3</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_TIM14</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_TIM15</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_TIM16</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_TIM17</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_SPI1</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_SPI2</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_USART1</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_USART2</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_I2C1</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_GPIOA</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_GPIOB</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_GPIOC</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_GPIOF</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_CRC</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_DMA1</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_SRAM</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_FLITF</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_WWDG</t>
-  </si>
-  <si>
-    <t>FMKCPU_RCC_CLK_PWR</t>
-  </si>
-  <si>
     <t>DMA_Name</t>
   </si>
   <si>
@@ -423,6 +354,144 @@
   </si>
   <si>
     <t>PA13</t>
+  </si>
+  <si>
+    <t>SYSCFG</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>TIM1</t>
+  </si>
+  <si>
+    <t>TIM3</t>
+  </si>
+  <si>
+    <t>TIM14</t>
+  </si>
+  <si>
+    <t>TIM15</t>
+  </si>
+  <si>
+    <t>TIM16</t>
+  </si>
+  <si>
+    <t>TIM17</t>
+  </si>
+  <si>
+    <t>SPI1</t>
+  </si>
+  <si>
+    <t>SPI2</t>
+  </si>
+  <si>
+    <t>USART1</t>
+  </si>
+  <si>
+    <t>USART2</t>
+  </si>
+  <si>
+    <t>I2C1</t>
+  </si>
+  <si>
+    <t>GPIOA</t>
+  </si>
+  <si>
+    <t>GPIOB</t>
+  </si>
+  <si>
+    <t>GPIOC</t>
+  </si>
+  <si>
+    <t>GPIOF</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>DMA1</t>
+  </si>
+  <si>
+    <t>SRAM</t>
+  </si>
+  <si>
+    <t>FLITF</t>
+  </si>
+  <si>
+    <t>WWDG</t>
+  </si>
+  <si>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>Clock for Global System configuration.</t>
+  </si>
+  <si>
+    <t>Clock for ADC1 register access.</t>
+  </si>
+  <si>
+    <t>Clock for Timer 1 register access.</t>
+  </si>
+  <si>
+    <t>Clock for Timer 3 register access.</t>
+  </si>
+  <si>
+    <t>Clock for Timer 14 register access.</t>
+  </si>
+  <si>
+    <t>Clock for Timer 15 register access.</t>
+  </si>
+  <si>
+    <t>Clock for Timer 16 register access.</t>
+  </si>
+  <si>
+    <t>Clock for Timer 17 register access.</t>
+  </si>
+  <si>
+    <t>Clock for SPI1 register access (Serial Peripheral Interface).</t>
+  </si>
+  <si>
+    <t>Clock for SPI2 register access (Serial Peripheral Interface).</t>
+  </si>
+  <si>
+    <t>Clock for USART1 register access (Universal Synchronous/Asynchronous Receiver/Transmitter).</t>
+  </si>
+  <si>
+    <t>Clock for USART2 register access (Universal Synchronous/Asynchronous Receiver/Transmitter).</t>
+  </si>
+  <si>
+    <t>Clock for I2C1 register access (Inter-Integrated Circuit).</t>
+  </si>
+  <si>
+    <t>Clock for GPIOA register access (General Purpose Input/Output A).</t>
+  </si>
+  <si>
+    <t>Clock for GPIOB register access (General Purpose Input/Output B).</t>
+  </si>
+  <si>
+    <t>Clock for GPIOC register access (General Purpose Input/Output C).</t>
+  </si>
+  <si>
+    <t>Clock for GPIOF register access (General Purpose Input/Output F).</t>
+  </si>
+  <si>
+    <t>Clock for CRC register access (Cyclic Redundancy Check).</t>
+  </si>
+  <si>
+    <t>Clock for DMA1 register access (Direct Memory Access).</t>
+  </si>
+  <si>
+    <t>Clock for SRAM register access (Static Random Access Memory).</t>
+  </si>
+  <si>
+    <t>Clock for Flash Interface register access.</t>
+  </si>
+  <si>
+    <t>Clock for Window Watchdog register access.</t>
+  </si>
+  <si>
+    <t>Clock for Power Control register access.</t>
   </si>
 </sst>
 </file>
@@ -971,14 +1040,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="C18:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E14" zoomScale="89" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="90" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+    <col min="4" max="4" width="81" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="33.109375" customWidth="1"/>
     <col min="7" max="7" width="20.77734375" customWidth="1"/>
@@ -986,8 +1055,11 @@
     <col min="9" max="9" width="21.33203125" customWidth="1"/>
     <col min="11" max="11" width="20.44140625" customWidth="1"/>
     <col min="12" max="12" width="17.44140625" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" customWidth="1"/>
     <col min="14" max="14" width="22.77734375" customWidth="1"/>
     <col min="15" max="15" width="23.44140625" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="18" spans="3:22" x14ac:dyDescent="0.3">
@@ -998,10 +1070,10 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="I18" t="s">
         <v>2</v>
@@ -1028,7 +1100,7 @@
         <v>19</v>
       </c>
       <c r="U18" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="V18" t="s">
         <v>19</v>
@@ -1036,13 +1108,16 @@
     </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>26</v>
+        <v>105</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I19" t="s">
         <v>4</v>
@@ -1077,13 +1152,16 @@
     </row>
     <row r="20" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>27</v>
+        <v>106</v>
+      </c>
+      <c r="D20" t="s">
+        <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I20" t="s">
         <v>5</v>
@@ -1100,13 +1178,16 @@
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>28</v>
+        <v>107</v>
+      </c>
+      <c r="D21" t="s">
+        <v>130</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="G21" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I21" t="s">
         <v>6</v>
@@ -1123,13 +1204,16 @@
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>29</v>
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="G22" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I22" t="s">
         <v>7</v>
@@ -1146,13 +1230,16 @@
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>30</v>
+        <v>109</v>
+      </c>
+      <c r="D23" t="s">
+        <v>132</v>
       </c>
       <c r="F23" t="s">
         <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I23" t="s">
         <v>8</v>
@@ -1169,13 +1256,16 @@
     </row>
     <row r="24" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>31</v>
+        <v>110</v>
+      </c>
+      <c r="D24" t="s">
+        <v>133</v>
       </c>
       <c r="F24" t="s">
         <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I24" t="s">
         <v>9</v>
@@ -1186,218 +1276,270 @@
     </row>
     <row r="25" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>32</v>
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>134</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="G25" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>33</v>
+        <v>112</v>
+      </c>
+      <c r="D26" t="s">
+        <v>135</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="G26" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>34</v>
+        <v>113</v>
+      </c>
+      <c r="D27" t="s">
+        <v>136</v>
       </c>
       <c r="F27" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G27" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>35</v>
+        <v>114</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
       </c>
       <c r="F28" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="G28" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>36</v>
+        <v>115</v>
+      </c>
+      <c r="D29" t="s">
+        <v>138</v>
       </c>
       <c r="F29" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="G29" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>37</v>
+        <v>116</v>
+      </c>
+      <c r="D30" t="s">
+        <v>139</v>
       </c>
       <c r="F30" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="G30" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>38</v>
+        <v>117</v>
+      </c>
+      <c r="D31" t="s">
+        <v>140</v>
       </c>
       <c r="F31" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="G31" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>39</v>
+        <v>118</v>
+      </c>
+      <c r="D32" t="s">
+        <v>141</v>
       </c>
       <c r="F32" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="G32" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>40</v>
+        <v>119</v>
+      </c>
+      <c r="D33" t="s">
+        <v>142</v>
       </c>
       <c r="F33" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="G33" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>41</v>
+        <v>120</v>
+      </c>
+      <c r="D34" t="s">
+        <v>143</v>
       </c>
       <c r="F34" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="G34" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>42</v>
+        <v>121</v>
+      </c>
+      <c r="D35" t="s">
+        <v>144</v>
       </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="G35" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>43</v>
+        <v>122</v>
+      </c>
+      <c r="D36" t="s">
+        <v>145</v>
       </c>
       <c r="F36" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="G36" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>44</v>
+        <v>123</v>
+      </c>
+      <c r="D37" t="s">
+        <v>146</v>
       </c>
       <c r="F37" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="G37" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>45</v>
+        <v>124</v>
+      </c>
+      <c r="D38" t="s">
+        <v>147</v>
       </c>
       <c r="F38" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="G38" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>46</v>
+        <v>125</v>
+      </c>
+      <c r="D39" t="s">
+        <v>148</v>
       </c>
       <c r="F39" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="G39" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>47</v>
+        <v>126</v>
+      </c>
+      <c r="D40" t="s">
+        <v>149</v>
       </c>
       <c r="F40" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="G40" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>48</v>
+        <v>127</v>
+      </c>
+      <c r="D41" t="s">
+        <v>150</v>
       </c>
       <c r="F41" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="G41" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F42" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="G42" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F43" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="G43" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="7">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1431,146 +1573,146 @@
   <sheetData>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="R4" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="W4" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="AD4" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="R5" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="S5" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="T5" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="U5" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="W5" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="X5" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="Y5" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="Z5" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="AA5" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="AB5" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="AD5" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="AE5" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="AF5" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="M6" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="N6" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="O6" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="P6" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="R6" t="s">
         <v>12</v>
       </c>
       <c r="S6" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="T6" t="s">
         <v>23</v>
       </c>
       <c r="U6" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="W6" t="s">
         <v>12</v>
       </c>
       <c r="X6" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="Y6" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="Z6" t="s">
         <v>6</v>
       </c>
       <c r="AA6" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="AB6" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="AD6" t="s">
         <v>12</v>
       </c>
       <c r="AE6" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="AF6" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
@@ -1578,82 +1720,82 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="K7" t="s">
         <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="M7" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N7" t="s">
         <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="P7" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="R7" t="s">
         <v>12</v>
       </c>
       <c r="S7" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="T7" t="s">
         <v>24</v>
       </c>
       <c r="U7" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="W7" t="s">
         <v>12</v>
       </c>
       <c r="X7" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="Y7" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="Z7" t="s">
         <v>7</v>
       </c>
       <c r="AA7" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="AB7" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="AD7" t="s">
         <v>12</v>
       </c>
       <c r="AE7" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="AF7" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
@@ -1661,70 +1803,70 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="K8" t="s">
         <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="M8" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="N8" t="s">
         <v>7</v>
       </c>
       <c r="O8" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="P8" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="W8" t="s">
         <v>12</v>
       </c>
       <c r="X8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y8" t="s">
         <v>54</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>77</v>
       </c>
       <c r="Z8" t="s">
         <v>7</v>
       </c>
       <c r="AA8" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="AB8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AD8" t="s">
         <v>12</v>
       </c>
       <c r="AE8" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="AF8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
@@ -1732,52 +1874,52 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="I9" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="K9" t="s">
         <v>12</v>
       </c>
       <c r="L9" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="M9" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="N9" t="s">
         <v>7</v>
       </c>
       <c r="O9" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="P9" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AD9" t="s">
         <v>12</v>
       </c>
       <c r="AE9" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="AF9" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
@@ -1785,19 +1927,19 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AD10" t="s">
         <v>13</v>
       </c>
       <c r="AE10" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="AF10" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
@@ -1805,19 +1947,19 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="AD11" t="s">
         <v>13</v>
       </c>
       <c r="AE11" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="AF11" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
@@ -1825,19 +1967,19 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="AD12" t="s">
         <v>13</v>
       </c>
       <c r="AE12" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="AF12" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
@@ -1845,19 +1987,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="AD13" t="s">
         <v>13</v>
       </c>
       <c r="AE13" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="AF13" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
@@ -1865,19 +2007,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="AD14" t="s">
         <v>13</v>
       </c>
       <c r="AE14" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="AF14" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
@@ -1885,19 +2027,19 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="AD15" t="s">
         <v>13</v>
       </c>
       <c r="AE15" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="AF15" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
@@ -1905,19 +2047,19 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="AD16" t="s">
         <v>13</v>
       </c>
       <c r="AE16" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="AF16" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
@@ -1925,19 +2067,19 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="AD17" t="s">
         <v>13</v>
       </c>
       <c r="AE17" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="AF17" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.3">
@@ -1945,19 +2087,19 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="AD18" t="s">
         <v>14</v>
       </c>
       <c r="AE18" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="AF18" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1980,14 +2122,14 @@
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -2003,7 +2145,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -2011,7 +2153,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CodeGen for module FMKCDA done
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbarb\Documents\PlatformIO\Projects\STM32_tplprj\Doc\ConfigPrj\ExcelCfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808D4FDA-0D0B-4C18-852F-36942223AFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C56ACA-09FC-4B52-BAE5-9ECC7E0B98BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_GPIO4" displayName="GI_GPIO4" ref="O18:P19" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="O18:P19" totalsRowShown="0">
   <autoFilter ref="O18:P19" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{46462DEE-B3A7-45AD-A2F8-63AC8C3C0154}" name="ADC_Name"/>
@@ -1040,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="C18:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="90" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="J10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,7 +1135,7 @@
         <v>17</v>
       </c>
       <c r="P19">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R19" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Work on Sig/ Timer/ adc/ channel Diagnostic
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbarb\Documents\PlatformIO\Projects\STM32_tplprj\Doc\ConfigPrj\ExcelCfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C56ACA-09FC-4B52-BAE5-9ECC7E0B98BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE591C1-FDEB-4E5E-8197-11B69265F5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="153">
   <si>
     <t>Colonne1</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>Clock for Power Control register access.</t>
+  </si>
+  <si>
+    <t>STM32 Family</t>
+  </si>
+  <si>
+    <t>STM32 Process</t>
   </si>
 </sst>
 </file>
@@ -553,8 +559,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}" name="GI_Timer" displayName="GI_Timer" ref="I18:J24" totalsRowShown="0">
-  <autoFilter ref="I18:J24" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}" name="GI_Timer" displayName="GI_Timer" ref="J18:K24" totalsRowShown="0">
+  <autoFilter ref="J18:K24" xr:uid="{82E1452B-3AF2-4D4B-B30D-A715E2B5240F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8EBC08AF-F674-4D3F-80D1-664693CE12C7}" name="Timer_name"/>
     <tableColumn id="2" xr3:uid="{9707AE90-9D0C-47B3-A89D-28A13CE83851}" name="Number of channels"/>
@@ -564,6 +570,18 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="AD5:AF18" totalsRowShown="0">
+  <autoFilter ref="AD5:AF18" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{395BD36A-0840-48CF-8D8D-56878E366FC5}" name="GPIO_name"/>
+    <tableColumn id="2" xr3:uid="{34DF2CF3-8826-4F9E-A09D-280EE0FEFFBB}" name="Pin_name"/>
+    <tableColumn id="3" xr3:uid="{E768A198-E65B-4C98-95AC-D8359662A49C}" name="bsp pin name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}" name="FMKIO_InputFreq" displayName="FMKIO_InputFreq" ref="K6:P9" totalsRowShown="0">
   <autoFilter ref="K6:P9" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}"/>
   <tableColumns count="6">
@@ -578,7 +596,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}" name="FMKIO_InputEvnt" displayName="FMKIO_InputEvnt" ref="R5:U7" totalsRowShown="0">
   <autoFilter ref="R5:U7" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}"/>
   <tableColumns count="4">
@@ -591,7 +609,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}" name="FMKIO_OutputPwm" displayName="FMKIO_OutputPwm" ref="W5:AB8" totalsRowShown="0">
   <autoFilter ref="W5:AB8" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}"/>
   <tableColumns count="6">
@@ -606,7 +624,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}" name="FMKIO_InputAna" displayName="FMKIO_InputAna" ref="E6:I9" totalsRowShown="0">
   <autoFilter ref="E6:I9" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}"/>
   <tableColumns count="5">
@@ -620,7 +638,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
@@ -632,8 +650,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}" name="GI_GPIO" displayName="GI_GPIO" ref="L18:M23" totalsRowShown="0">
-  <autoFilter ref="L18:M23" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}" name="GI_GPIO" displayName="GI_GPIO" ref="M18:N23" totalsRowShown="0">
+  <autoFilter ref="M18:N23" xr:uid="{FB0F4D34-CEA0-4CC8-AB6D-4C40C7CBEB5D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3404615A-1121-4984-AE0D-5A1D34461BCA}" name="GPIO_Name"/>
     <tableColumn id="2" xr3:uid="{37ECDCD3-2CED-4177-80B2-3A88EFA9E7C2}" name="Number of pin"/>
@@ -643,8 +661,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="O18:P19" totalsRowShown="0">
-  <autoFilter ref="O18:P19" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}" name="GI_ADC" displayName="GI_ADC" ref="P18:Q19" totalsRowShown="0">
+  <autoFilter ref="P18:Q19" xr:uid="{A27CADD5-26F4-4DF6-9D41-CEE02A85C4E9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{46462DEE-B3A7-45AD-A2F8-63AC8C3C0154}" name="ADC_Name"/>
     <tableColumn id="2" xr3:uid="{20DF5352-4B39-416D-A6E4-D94E56AED1C9}" name="number of channel"/>
@@ -654,8 +672,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="R18:S19" totalsRowShown="0">
-  <autoFilter ref="R18:S19" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}" name="GI_DAC" displayName="GI_DAC" ref="S18:T19" totalsRowShown="0">
+  <autoFilter ref="S18:T19" xr:uid="{5A8C957F-EDE6-44F1-B8F8-2086E255196A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{73150C50-6B2A-4CD8-A7E6-62C171935AF8}" name="DAC_Name"/>
     <tableColumn id="2" xr3:uid="{EF9B5413-9A3C-4163-8063-C74DAB2D51F7}" name="number of channel"/>
@@ -665,8 +683,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0BD818BF-294B-4FA2-8E5A-7FD1DB70B357}" name="GI_IRQN" displayName="GI_IRQN" ref="F18:G43" totalsRowShown="0">
-  <autoFilter ref="F18:G43" xr:uid="{0BD818BF-294B-4FA2-8E5A-7FD1DB70B357}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0BD818BF-294B-4FA2-8E5A-7FD1DB70B357}" name="GI_IRQN" displayName="GI_IRQN" ref="G18:H43" totalsRowShown="0">
+  <autoFilter ref="G18:H43" xr:uid="{0BD818BF-294B-4FA2-8E5A-7FD1DB70B357}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{95486269-8ABF-444C-A7FD-956C784AC88B}" name="IRQN_name"/>
     <tableColumn id="2" xr3:uid="{72C5AB1D-5859-4FB9-812E-7971E444E4B8}" name="Interrupt Prioirty "/>
@@ -676,8 +694,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}" name="GI_RCC_CLOCK" displayName="GI_RCC_CLOCK" ref="C18:D41" totalsRowShown="0">
-  <autoFilter ref="C18:D41" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}" name="GI_RCC_CLOCK" displayName="GI_RCC_CLOCK" ref="D18:E41" totalsRowShown="0">
+  <autoFilter ref="D18:E41" xr:uid="{9B4F1398-0B6D-4B55-A4C3-611E0B66A012}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{402A3AD5-0AFA-40A5-A5A4-0D9CB2EED72D}" name="RCC_ClockName"/>
     <tableColumn id="2" xr3:uid="{05025EF0-98DC-4B06-8DD6-ABD9D73D50B7}" name="Description"/>
@@ -687,8 +705,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="U18:V19" totalsRowShown="0">
-  <autoFilter ref="U18:V19" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}" name="GI_DMA" displayName="GI_DMA" ref="V18:W19" totalsRowShown="0">
+  <autoFilter ref="V18:W19" xr:uid="{FC2F87AB-FFF7-4006-99CC-8D938E27338D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00302DEC-D815-47CE-9380-676FE769FF43}" name="DMA_Name"/>
     <tableColumn id="2" xr3:uid="{2654BB85-F763-4BBA-9124-13A3875B62D0}" name="number of channel"/>
@@ -698,24 +716,23 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{69B16F87-38FA-4931-845E-91EC8B0FFB29}" name="Tableau5" displayName="Tableau5" ref="A15:B16" totalsRowShown="0">
+  <autoFilter ref="A15:B16" xr:uid="{69B16F87-38FA-4931-845E-91EC8B0FFB29}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FD4FECA3-1A39-43C0-8443-3217FDF815FF}" name="STM32 Family"/>
+    <tableColumn id="2" xr3:uid="{DDA90C22-9D42-40D5-A8DF-C1879E8D680C}" name="STM32 Process"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}" name="FMKIO_InputDig" displayName="FMKIO_InputDig" ref="A6:C18" totalsRowShown="0">
   <autoFilter ref="A6:C18" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6C4BEFED-5E85-401A-AA66-51A07D13FEBC}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{E08F986F-8D6D-4DEB-A18F-F4FB9A36C956}" name="Pin_name"/>
     <tableColumn id="3" xr3:uid="{F49EBA6C-41BD-4C20-9D26-15768A7B10D2}" name="bsp pin name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="AD5:AF18" totalsRowShown="0">
-  <autoFilter ref="AD5:AF18" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{395BD36A-0840-48CF-8D8D-56878E366FC5}" name="GPIO_name"/>
-    <tableColumn id="2" xr3:uid="{34DF2CF3-8826-4F9E-A09D-280EE0FEFFBB}" name="Pin_name"/>
-    <tableColumn id="3" xr3:uid="{E768A198-E65B-4C98-95AC-D8359662A49C}" name="bsp pin name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1038,14 +1055,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
-  <dimension ref="C18:V43"/>
+  <dimension ref="A15:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="81" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
@@ -1062,469 +1081,477 @@
     <col min="19" max="19" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>22</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>64</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>65</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>2</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>3</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>10</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>11</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>18</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>19</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>20</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>19</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>26</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+    <row r="19" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
         <v>105</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>128</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>66</v>
       </c>
-      <c r="G19" t="s">
-        <v>89</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="H19" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" t="s">
         <v>4</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>4</v>
       </c>
-      <c r="L19" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19">
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19">
         <v>16</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>17</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>18</v>
-      </c>
-      <c r="R19" t="s">
-        <v>21</v>
       </c>
       <c r="S19" t="s">
         <v>21</v>
       </c>
-      <c r="U19" t="s">
+      <c r="T19" t="s">
         <v>21</v>
       </c>
       <c r="V19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="W19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
         <v>106</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>129</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>67</v>
       </c>
-      <c r="G20" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="H20" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" t="s">
         <v>5</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>4</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>13</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+    <row r="21" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
         <v>107</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>130</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>68</v>
       </c>
-      <c r="G21" t="s">
-        <v>89</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="H21" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" t="s">
         <v>6</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>14</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+    <row r="22" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
         <v>108</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>131</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>69</v>
       </c>
-      <c r="G22" t="s">
-        <v>89</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="H22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J22" t="s">
         <v>7</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>2</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>15</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
+    <row r="23" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
         <v>109</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>132</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>23</v>
       </c>
-      <c r="G23" t="s">
-        <v>89</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="H23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" t="s">
         <v>8</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>1</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>16</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
+    <row r="24" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
         <v>110</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>133</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>24</v>
       </c>
-      <c r="G24" t="s">
-        <v>89</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="H24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" t="s">
         <v>9</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
+    <row r="25" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
         <v>111</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>134</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>70</v>
       </c>
-      <c r="G25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
+      <c r="H25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
         <v>112</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>135</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>71</v>
       </c>
-      <c r="G26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
         <v>113</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>136</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>72</v>
       </c>
-      <c r="G27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
+      <c r="H27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
         <v>114</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>137</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>73</v>
       </c>
-      <c r="G28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
+      <c r="H28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
         <v>115</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>138</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="G29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
+      <c r="H29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
         <v>116</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>139</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>75</v>
       </c>
-      <c r="G30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
+      <c r="H30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
         <v>117</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>140</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>76</v>
       </c>
-      <c r="G31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
+      <c r="H31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
         <v>118</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>141</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>77</v>
       </c>
-      <c r="G32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
+      <c r="H32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
         <v>119</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>142</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>78</v>
       </c>
-      <c r="G33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
+      <c r="H33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
         <v>120</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>143</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>79</v>
       </c>
-      <c r="G34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
+      <c r="H34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
         <v>121</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>144</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>80</v>
       </c>
-      <c r="G35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
+      <c r="H35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
         <v>122</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>145</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>81</v>
       </c>
-      <c r="G36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
+      <c r="H36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
         <v>123</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>146</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>82</v>
       </c>
-      <c r="G37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
+      <c r="H37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
         <v>124</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>147</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>83</v>
       </c>
-      <c r="G38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
+      <c r="H38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
         <v>125</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>148</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>84</v>
       </c>
-      <c r="G39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
+      <c r="H39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
         <v>126</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>149</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>85</v>
       </c>
-      <c r="G40" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
+      <c r="H40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
         <v>127</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>150</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>86</v>
       </c>
-      <c r="G41" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F42" t="s">
+      <c r="H41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
         <v>87</v>
       </c>
-      <c r="G42" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F43" t="s">
+      <c r="H42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="G43" t="s">
         <v>88</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1532,7 +1559,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="7">
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1540,6 +1567,7 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Work on excel configuration
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbarb\Documents\PlatformIO\Projects\STM32_tplprj\Doc\ConfigPrj\ExcelCfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE591C1-FDEB-4E5E-8197-11B69265F5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C40DA0B-2379-410E-9122-1D8485E4E7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="191">
   <si>
     <t>Colonne1</t>
   </si>
@@ -314,9 +314,6 @@
     <t>bsp pin name</t>
   </si>
   <si>
-    <t>PA0</t>
-  </si>
-  <si>
     <t>PA1</t>
   </si>
   <si>
@@ -498,6 +495,123 @@
   </si>
   <si>
     <t>STM32 Process</t>
+  </si>
+  <si>
+    <t>_NVIC_Piority_Choice</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>Pin_Choice</t>
+  </si>
+  <si>
+    <t>CHANNEL_3</t>
+  </si>
+  <si>
+    <t>Channel_Choice</t>
+  </si>
+  <si>
+    <t>PC6</t>
+  </si>
+  <si>
+    <t>PC7</t>
+  </si>
+  <si>
+    <t>PC8</t>
+  </si>
+  <si>
+    <t>PC9</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_0</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_1</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_2</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_3</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_4</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_5</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_6</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_7</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_8</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_9</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_10</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_11</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_12</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_13</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_14</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_15</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_16</t>
+  </si>
+  <si>
+    <t>ADC_CHANNEL_17</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC0</t>
+  </si>
+  <si>
+    <t>PB8</t>
+  </si>
+  <si>
+    <t>PB9</t>
+  </si>
+  <si>
+    <t>PB15</t>
+  </si>
+  <si>
+    <t>PB14</t>
+  </si>
+  <si>
+    <t>EXT1_3IRQN</t>
+  </si>
+  <si>
+    <t>PF1</t>
+  </si>
+  <si>
+    <t>PF0</t>
   </si>
 </sst>
 </file>
@@ -570,6 +684,18 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}" name="FMKIO_InputDig" displayName="FMKIO_InputDig" ref="A6:C18" totalsRowShown="0">
+  <autoFilter ref="A6:C18" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6C4BEFED-5E85-401A-AA66-51A07D13FEBC}" name="GPIO_name"/>
+    <tableColumn id="2" xr3:uid="{E08F986F-8D6D-4DEB-A18F-F4FB9A36C956}" name="Pin_name"/>
+    <tableColumn id="3" xr3:uid="{F49EBA6C-41BD-4C20-9D26-15768A7B10D2}" name="bsp pin name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}" name="FMKIO_OutputDig" displayName="FMKIO_OutputDig" ref="AD5:AF18" totalsRowShown="0">
   <autoFilter ref="AD5:AF18" xr:uid="{098A48DC-88A9-4122-ADE1-86E0F3796141}"/>
   <tableColumns count="3">
@@ -581,7 +707,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}" name="FMKIO_InputFreq" displayName="FMKIO_InputFreq" ref="K6:P9" totalsRowShown="0">
   <autoFilter ref="K6:P9" xr:uid="{27D0C574-E325-48F5-AA31-7FBAF1E09007}"/>
   <tableColumns count="6">
@@ -596,7 +722,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}" name="FMKIO_InputEvnt" displayName="FMKIO_InputEvnt" ref="R5:U7" totalsRowShown="0">
   <autoFilter ref="R5:U7" xr:uid="{0918A5C3-EE53-4DBF-8C0C-2251FB41871E}"/>
   <tableColumns count="4">
@@ -609,9 +735,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}" name="FMKIO_OutputPwm" displayName="FMKIO_OutputPwm" ref="W5:AB8" totalsRowShown="0">
-  <autoFilter ref="W5:AB8" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}"/>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}" name="FMKIO_OutputPwm" displayName="FMKIO_OutputPwm" ref="W5:AB13" totalsRowShown="0">
+  <autoFilter ref="W5:AB13" xr:uid="{DE41CD30-BCBD-40FE-B5DD-848DAAA9C25B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{F2B685DB-87AE-429A-9E70-076DA856F9A2}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{30126296-E33C-4D56-9110-2D49FE159CF1}" name="Pin_name"/>
@@ -624,9 +750,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}" name="FMKIO_InputAna" displayName="FMKIO_InputAna" ref="E6:I9" totalsRowShown="0">
-  <autoFilter ref="E6:I9" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}"/>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}" name="FMKIO_InputAna" displayName="FMKIO_InputAna" ref="E6:I17" totalsRowShown="0">
+  <autoFilter ref="E6:I17" xr:uid="{B6D8F853-4E95-4D0E-932E-0F3ECC221901}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EDBDBF14-1FA4-44B8-A62D-BAA9F312652A}" name="GPIO_name"/>
     <tableColumn id="2" xr3:uid="{75AD9B1E-8F88-4CD9-86AB-C0D6BFDB44CD}" name="Pin_name"/>
@@ -638,7 +764,37 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3EEFA786-828B-422C-9405-D0B0DD120CF4}" name="Tableau17" displayName="Tableau17" ref="AJ5:AJ21" totalsRowShown="0">
+  <autoFilter ref="AJ5:AJ21" xr:uid="{3EEFA786-828B-422C-9405-D0B0DD120CF4}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{01BF5210-733A-4DB1-A72E-FC1B749F7F18}" name="Pin_Choice"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}" name="Tableau18" displayName="Tableau18" ref="AL6:AL10" totalsRowShown="0">
+  <autoFilter ref="AL6:AL10" xr:uid="{06E0084F-32F1-4C7D-A6E0-EE7152DB4CBF}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{DD976920-6FFB-4C96-8085-12D970F3A0A7}" name="Channel_Choice"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}" name="Tableau1720" displayName="Tableau1720" ref="AN5:AN23" totalsRowShown="0">
+  <autoFilter ref="AN5:AN23" xr:uid="{9F1C0A09-0E71-42DD-A451-D3B53F431EBF}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{D50D0836-4115-4278-AA16-2E66D5FB62AC}" name="Adc_Channel"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
   <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
   <tableColumns count="2">
@@ -727,12 +883,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}" name="FMKIO_InputDig" displayName="FMKIO_InputDig" ref="A6:C18" totalsRowShown="0">
-  <autoFilter ref="A6:C18" xr:uid="{9F4B7C8E-8730-4908-B1BE-2954AF9427C0}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6C4BEFED-5E85-401A-AA66-51A07D13FEBC}" name="GPIO_name"/>
-    <tableColumn id="2" xr3:uid="{E08F986F-8D6D-4DEB-A18F-F4FB9A36C956}" name="Pin_name"/>
-    <tableColumn id="3" xr3:uid="{F49EBA6C-41BD-4C20-9D26-15768A7B10D2}" name="bsp pin name"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AA17:AA20" totalsRowShown="0">
+  <autoFilter ref="AA17:AA20" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{84137467-8FB1-43EA-9F20-573D7FE9FADD}" name="_NVIC_Piority_Choice"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1055,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
-  <dimension ref="A15:W43"/>
+  <dimension ref="A15:AA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="G9" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,9 +1221,9 @@
     <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="81" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="85.109375" customWidth="1"/>
     <col min="6" max="6" width="33.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" customWidth="1"/>
     <col min="8" max="8" width="21.44140625" customWidth="1"/>
     <col min="9" max="9" width="21.33203125" customWidth="1"/>
     <col min="11" max="11" width="20.44140625" customWidth="1"/>
@@ -1079,17 +1233,25 @@
     <col min="15" max="15" width="23.44140625" customWidth="1"/>
     <col min="16" max="16" width="20.6640625" customWidth="1"/>
     <col min="19" max="19" width="21.33203125" customWidth="1"/>
+    <col min="22" max="22" width="18.77734375" customWidth="1"/>
+    <col min="23" max="23" width="29.21875" customWidth="1"/>
+    <col min="27" max="27" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="17" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="AA17" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>25</v>
       </c>
@@ -1132,13 +1294,16 @@
       <c r="W18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="AA18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G19" t="s">
         <v>66</v>
@@ -1176,13 +1341,16 @@
       <c r="W19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="AA19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G20" t="s">
         <v>67</v>
@@ -1202,13 +1370,16 @@
       <c r="N20">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="AA20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G21" t="s">
         <v>68</v>
@@ -1229,12 +1400,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G22" t="s">
         <v>69</v>
@@ -1255,12 +1426,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G23" t="s">
         <v>23</v>
@@ -1281,12 +1452,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G24" t="s">
         <v>24</v>
@@ -1301,12 +1472,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G25" t="s">
         <v>70</v>
@@ -1315,12 +1486,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G26" t="s">
         <v>71</v>
@@ -1329,12 +1500,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G27" t="s">
         <v>72</v>
@@ -1343,12 +1514,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G28" t="s">
         <v>73</v>
@@ -1357,12 +1528,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G29" t="s">
         <v>74</v>
@@ -1371,12 +1542,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G30" t="s">
         <v>75</v>
@@ -1385,12 +1556,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G31" t="s">
         <v>76</v>
@@ -1399,12 +1570,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="4:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G32" t="s">
         <v>77</v>
@@ -1415,10 +1586,10 @@
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G33" t="s">
         <v>78</v>
@@ -1429,10 +1600,10 @@
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G34" t="s">
         <v>79</v>
@@ -1443,10 +1614,10 @@
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G35" t="s">
         <v>80</v>
@@ -1457,10 +1628,10 @@
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G36" t="s">
         <v>81</v>
@@ -1471,10 +1642,10 @@
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G37" t="s">
         <v>82</v>
@@ -1485,10 +1656,10 @@
     </row>
     <row r="38" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G38" t="s">
         <v>83</v>
@@ -1499,10 +1670,10 @@
     </row>
     <row r="39" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G39" t="s">
         <v>84</v>
@@ -1513,10 +1684,10 @@
     </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G40" t="s">
         <v>85</v>
@@ -1527,10 +1698,10 @@
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G41" t="s">
         <v>86</v>
@@ -1559,7 +1730,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="8">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1568,16 +1739,17 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
-  <dimension ref="A4:AF18"/>
+  <dimension ref="A4:AN23"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="P2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1590,6 +1762,7 @@
     <col min="8" max="8" width="17.33203125" customWidth="1"/>
     <col min="9" max="9" width="15.21875" customWidth="1"/>
     <col min="10" max="10" width="24.109375" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" customWidth="1"/>
     <col min="16" max="16" width="24.6640625" customWidth="1"/>
     <col min="18" max="18" width="14.88671875" customWidth="1"/>
     <col min="20" max="20" width="18.44140625" customWidth="1"/>
@@ -1597,9 +1770,11 @@
     <col min="25" max="25" width="16.77734375" customWidth="1"/>
     <col min="27" max="27" width="16.77734375" customWidth="1"/>
     <col min="31" max="31" width="17.6640625" customWidth="1"/>
+    <col min="38" max="38" width="17.21875" customWidth="1"/>
+    <col min="40" max="40" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="R4" t="s">
         <v>62</v>
       </c>
@@ -1610,7 +1785,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1659,8 +1834,14 @@
       <c r="AF5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AJ5" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1704,34 +1885,34 @@
         <v>90</v>
       </c>
       <c r="R6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S6" t="s">
         <v>29</v>
       </c>
       <c r="T6" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="U6" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="W6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="X6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="Y6" t="s">
         <v>54</v>
       </c>
       <c r="Z6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA6" t="s">
         <v>51</v>
       </c>
       <c r="AB6" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="AD6" t="s">
         <v>12</v>
@@ -1740,21 +1921,30 @@
         <v>42</v>
       </c>
       <c r="AF6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
         <v>29</v>
@@ -1763,16 +1953,16 @@
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="I7" t="s">
-        <v>92</v>
+        <v>183</v>
       </c>
       <c r="K7" t="s">
         <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="M7" t="s">
         <v>49</v>
@@ -1784,37 +1974,37 @@
         <v>51</v>
       </c>
       <c r="P7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="R7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S7" t="s">
         <v>30</v>
       </c>
       <c r="T7" t="s">
-        <v>24</v>
+        <v>188</v>
       </c>
       <c r="U7" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
       <c r="W7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="X7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="Y7" t="s">
         <v>54</v>
       </c>
       <c r="Z7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AA7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AB7" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="AD7" t="s">
         <v>12</v>
@@ -1823,10 +2013,19 @@
         <v>43</v>
       </c>
       <c r="AF7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1834,10 +2033,10 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
@@ -1846,16 +2045,16 @@
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>173</v>
       </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>182</v>
       </c>
       <c r="K8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L8" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="M8" t="s">
         <v>50</v>
@@ -1867,25 +2066,25 @@
         <v>51</v>
       </c>
       <c r="P8" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="W8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="X8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="Y8" t="s">
         <v>54</v>
       </c>
       <c r="Z8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AA8" t="s">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="AB8" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="AD8" t="s">
         <v>12</v>
@@ -1894,10 +2093,19 @@
         <v>44</v>
       </c>
       <c r="AF8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1905,10 +2113,10 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
         <v>31</v>
@@ -1917,16 +2125,16 @@
         <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>181</v>
       </c>
       <c r="K9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L9" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="M9" t="s">
         <v>50</v>
@@ -1938,7 +2146,25 @@
         <v>52</v>
       </c>
       <c r="P9" t="s">
-        <v>94</v>
+        <v>186</v>
+      </c>
+      <c r="W9" t="s">
+        <v>14</v>
+      </c>
+      <c r="X9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>161</v>
       </c>
       <c r="AD9" t="s">
         <v>12</v>
@@ -1947,10 +2173,19 @@
         <v>45</v>
       </c>
       <c r="AF9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1958,7 +2193,40 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" t="s">
+        <v>180</v>
+      </c>
+      <c r="W10" t="s">
+        <v>12</v>
+      </c>
+      <c r="X10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>98</v>
       </c>
       <c r="AD10" t="s">
         <v>13</v>
@@ -1967,10 +2235,19 @@
         <v>31</v>
       </c>
       <c r="AF10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1978,7 +2255,40 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" t="s">
+        <v>96</v>
+      </c>
+      <c r="W11" t="s">
+        <v>12</v>
+      </c>
+      <c r="X11" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>99</v>
       </c>
       <c r="AD11" t="s">
         <v>13</v>
@@ -1987,10 +2297,16 @@
         <v>32</v>
       </c>
       <c r="AF11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1998,7 +2314,40 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>169</v>
+      </c>
+      <c r="I12" t="s">
+        <v>97</v>
+      </c>
+      <c r="W12" t="s">
+        <v>12</v>
+      </c>
+      <c r="X12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>100</v>
       </c>
       <c r="AD12" t="s">
         <v>13</v>
@@ -2007,10 +2356,16 @@
         <v>33</v>
       </c>
       <c r="AF12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2018,7 +2373,40 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" t="s">
+        <v>184</v>
+      </c>
+      <c r="W13" t="s">
+        <v>12</v>
+      </c>
+      <c r="X13" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>101</v>
       </c>
       <c r="AD13" t="s">
         <v>13</v>
@@ -2027,10 +2415,16 @@
         <v>34</v>
       </c>
       <c r="AF13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2038,7 +2432,22 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>171</v>
+      </c>
+      <c r="I14" t="s">
+        <v>185</v>
       </c>
       <c r="AD14" t="s">
         <v>13</v>
@@ -2047,10 +2456,16 @@
         <v>39</v>
       </c>
       <c r="AF14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2058,7 +2473,22 @@
         <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I15" t="s">
+        <v>91</v>
       </c>
       <c r="AD15" t="s">
         <v>13</v>
@@ -2067,10 +2497,16 @@
         <v>40</v>
       </c>
       <c r="AF15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2078,7 +2514,22 @@
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>164</v>
+      </c>
+      <c r="I16" t="s">
+        <v>92</v>
       </c>
       <c r="AD16" t="s">
         <v>13</v>
@@ -2087,10 +2538,16 @@
         <v>42</v>
       </c>
       <c r="AF16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2098,7 +2555,22 @@
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
+        <v>165</v>
+      </c>
+      <c r="I17" t="s">
+        <v>93</v>
       </c>
       <c r="AD17" t="s">
         <v>13</v>
@@ -2107,10 +2579,16 @@
         <v>43</v>
       </c>
       <c r="AF17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2118,7 +2596,7 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AD18" t="s">
         <v>14</v>
@@ -2127,21 +2605,93 @@
         <v>43</v>
       </c>
       <c r="AF18" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AJ19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AJ20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AJ21" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AN22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AN23" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ22 B7:B18 F7:F17 L7:L9 S6:S7 X6:X13 AE6:AE18" xr:uid="{14BC2D73-1395-4E2C-9D1E-55C781825C64}">
+      <formula1>$AJ$6:$AJ$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA13 O7:O9" xr:uid="{727A5344-B28A-4866-9EC1-7C96029AF8B6}">
+      <formula1>$AL$7:$AL$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H17" xr:uid="{FFFA1AF2-B35F-4BAA-AEF6-4A6121806F8D}">
+      <formula1>$AN$6:$AN$23</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="6">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA00DA78-9682-47F8-B701-D35809CE3FB0}">
+          <x14:formula1>
+            <xm:f>General_Info!$M$19:$M$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>A7:A18 E7:E17 K7:K9 R6:R7 W6:W13 AD6:AD18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C3D18C3-7241-4088-8034-07AAE0EB53A9}">
+          <x14:formula1>
+            <xm:f>General_Info!$J$19:$J$24</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z6:Z13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2150,7 +2700,7 @@
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Work on FMKMAC module
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/Hardware_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbarb\Documents\PlatformIO\Projects\STM32_tplprj\Doc\ConfigPrj\ExcelCfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C40DA0B-2379-410E-9122-1D8485E4E7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95097A0-0B2B-4E34-8347-11DF1030CEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="223">
   <si>
     <t>Colonne1</t>
   </si>
@@ -605,13 +605,109 @@
     <t>PB14</t>
   </si>
   <si>
-    <t>EXT1_3IRQN</t>
-  </si>
-  <si>
     <t>PF1</t>
   </si>
   <si>
     <t>PF0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Others SPI configuration</t>
+  </si>
+  <si>
+    <t>Bsp_Pin_Name</t>
+  </si>
+  <si>
+    <t>Others I2C  configuration</t>
+  </si>
+  <si>
+    <t>PB6</t>
+  </si>
+  <si>
+    <t>PB7</t>
+  </si>
+  <si>
+    <t>PC10</t>
+  </si>
+  <si>
+    <t>PC11</t>
+  </si>
+  <si>
+    <t>PC12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others USART _1 configuration (USART4 in DataSheet) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others USART _2 configuration (USART1 in DataSheet) </t>
+  </si>
+  <si>
+    <t>PA0</t>
+  </si>
+  <si>
+    <t>PA14</t>
+  </si>
+  <si>
+    <t>PA15</t>
+  </si>
+  <si>
+    <t>PB0</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>PB2</t>
+  </si>
+  <si>
+    <t>PB3</t>
+  </si>
+  <si>
+    <t>PB4</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>PB10</t>
+  </si>
+  <si>
+    <t>PB11</t>
+  </si>
+  <si>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>PC5</t>
+  </si>
+  <si>
+    <t>PC13</t>
+  </si>
+  <si>
+    <t>PC14</t>
+  </si>
+  <si>
+    <t>PC15</t>
+  </si>
+  <si>
+    <t>PF4</t>
+  </si>
+  <si>
+    <t>PF5</t>
+  </si>
+  <si>
+    <t>PF6</t>
+  </si>
+  <si>
+    <t>PF7</t>
   </si>
 </sst>
 </file>
@@ -795,11 +891,12 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
-  <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B097540B-A2DD-432F-8D25-C369E6A041DD}" name="Colonne1"/>
-    <tableColumn id="2" xr3:uid="{B680C179-8637-4CB0-847E-6E544634DED3}" name="Colonne2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}" name="Tableau20" displayName="Tableau20" ref="A26:C29" totalsRowShown="0">
+  <autoFilter ref="A26:C29" xr:uid="{B3BFFBC0-5215-4824-AE53-6F0674E6F949}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{35492CF7-2D64-4A31-B52A-8DC201862D23}" name="GPIO_name"/>
+    <tableColumn id="2" xr3:uid="{55201EA4-78EC-451A-894D-4121BE7C2D46}" name="Pin_name"/>
+    <tableColumn id="3" xr3:uid="{95976D38-4750-4385-89A0-E867F26709DF}" name="Bsp_Pin_Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -811,6 +908,53 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3404615A-1121-4984-AE0D-5A1D34461BCA}" name="GPIO_Name"/>
     <tableColumn id="2" xr3:uid="{37ECDCD3-2CED-4177-80B2-3A88EFA9E7C2}" name="Number of pin"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}" name="Tableau2022" displayName="Tableau2022" ref="E27:G29" totalsRowShown="0">
+  <autoFilter ref="E27:G29" xr:uid="{0C2EE56A-0FA0-4A8F-A981-3DF80A8100DC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{231389D4-B645-4CB2-A30E-5CBE9EE6FEFC}" name="GPIO_name"/>
+    <tableColumn id="2" xr3:uid="{56336DBF-18EC-4309-B422-97BDC37985D4}" name="Pin_name"/>
+    <tableColumn id="3" xr3:uid="{1167559C-5083-4ABC-8F8C-8F11E7C7FAA7}" name="Bsp_Pin_Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}" name="Tableau202223" displayName="Tableau202223" ref="I27:K30" totalsRowShown="0">
+  <autoFilter ref="I27:K30" xr:uid="{EB071486-BBE3-47FA-A4DE-38B8C83448BA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{30F87F4B-0EBB-4470-919C-8CEF7288D9C8}" name="GPIO_name"/>
+    <tableColumn id="2" xr3:uid="{DAB30C64-2E65-452D-A80D-3D932E8F35B6}" name="Pin_name"/>
+    <tableColumn id="3" xr3:uid="{5633DAA7-5910-4D39-A1CD-689650D5DAF3}" name="Bsp_Pin_Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}" name="Tableau20222324" displayName="Tableau20222324" ref="M27:O30" totalsRowShown="0">
+  <autoFilter ref="M27:O30" xr:uid="{0413BBED-76B8-4200-A43C-D97EFAA1EA94}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{95762CE8-B06D-493C-B844-88501CD65909}" name="GPIO_name"/>
+    <tableColumn id="2" xr3:uid="{F5525426-5A61-46C9-A36F-3B7B9F70AC40}" name="Pin_name"/>
+    <tableColumn id="3" xr3:uid="{108F58E5-A0A9-420E-87F0-F24D6540D066}" name="Bsp_Pin_Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}" name="FMKCPU_EvntTimer" displayName="FMKCPU_EvntTimer" ref="B4:C6" totalsRowShown="0">
+  <autoFilter ref="B4:C6" xr:uid="{684AB3A4-4693-477C-AADC-64EBB335C3E9}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B097540B-A2DD-432F-8D25-C369E6A041DD}" name="Colonne1"/>
+    <tableColumn id="2" xr3:uid="{B680C179-8637-4CB0-847E-6E544634DED3}" name="Colonne2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1746,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492C7761-01BE-400F-9C40-BE71D85F5C61}">
-  <dimension ref="A4:AN23"/>
+  <dimension ref="A4:AN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE23" sqref="AE23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1759,6 +1903,7 @@
     <col min="3" max="3" width="19.5546875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" customWidth="1"/>
     <col min="9" max="9" width="15.21875" customWidth="1"/>
     <col min="10" max="10" width="24.109375" customWidth="1"/>
@@ -1769,6 +1914,7 @@
     <col min="24" max="24" width="20" customWidth="1"/>
     <col min="25" max="25" width="16.77734375" customWidth="1"/>
     <col min="27" max="27" width="16.77734375" customWidth="1"/>
+    <col min="30" max="30" width="13" customWidth="1"/>
     <col min="31" max="31" width="17.6640625" customWidth="1"/>
     <col min="38" max="38" width="17.21875" customWidth="1"/>
     <col min="40" max="40" width="19.44140625" customWidth="1"/>
@@ -1891,10 +2037,10 @@
         <v>29</v>
       </c>
       <c r="T6" t="s">
-        <v>188</v>
+        <v>23</v>
       </c>
       <c r="U6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="W6" t="s">
         <v>14</v>
@@ -1915,13 +2061,13 @@
         <v>158</v>
       </c>
       <c r="AD6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AE6" t="s">
         <v>42</v>
       </c>
       <c r="AF6" t="s">
-        <v>91</v>
+        <v>212</v>
       </c>
       <c r="AJ6" t="s">
         <v>29</v>
@@ -1935,13 +2081,13 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1983,10 +2129,10 @@
         <v>30</v>
       </c>
       <c r="T7" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" t="s">
         <v>188</v>
-      </c>
-      <c r="U7" t="s">
-        <v>189</v>
       </c>
       <c r="W7" t="s">
         <v>14</v>
@@ -2007,13 +2153,13 @@
         <v>159</v>
       </c>
       <c r="AD7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AE7" t="s">
         <v>43</v>
       </c>
       <c r="AF7" t="s">
-        <v>92</v>
+        <v>213</v>
       </c>
       <c r="AJ7" t="s">
         <v>30</v>
@@ -2030,10 +2176,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -2087,13 +2233,13 @@
         <v>160</v>
       </c>
       <c r="AD8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AE8" t="s">
         <v>44</v>
       </c>
       <c r="AF8" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="AJ8" t="s">
         <v>31</v>
@@ -2110,10 +2256,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -2167,13 +2313,13 @@
         <v>161</v>
       </c>
       <c r="AD9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AE9" t="s">
         <v>45</v>
       </c>
       <c r="AF9" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="AJ9" t="s">
         <v>32</v>
@@ -2190,10 +2336,10 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>203</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -2229,13 +2375,13 @@
         <v>98</v>
       </c>
       <c r="AD10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AF10" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="AJ10" t="s">
         <v>33</v>
@@ -2249,13 +2395,13 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>204</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -2291,13 +2437,13 @@
         <v>99</v>
       </c>
       <c r="AD11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AF11" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="AJ11" t="s">
         <v>34</v>
@@ -2308,13 +2454,13 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>205</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -2331,6 +2477,9 @@
       <c r="I12" t="s">
         <v>97</v>
       </c>
+      <c r="T12" t="s">
+        <v>190</v>
+      </c>
       <c r="W12" t="s">
         <v>12</v>
       </c>
@@ -2350,13 +2499,13 @@
         <v>100</v>
       </c>
       <c r="AD12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE12" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="AF12" t="s">
-        <v>97</v>
+        <v>216</v>
       </c>
       <c r="AJ12" t="s">
         <v>35</v>
@@ -2367,13 +2516,13 @@
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -2409,13 +2558,13 @@
         <v>101</v>
       </c>
       <c r="AD13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE13" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="AF13" t="s">
-        <v>98</v>
+        <v>217</v>
       </c>
       <c r="AJ13" t="s">
         <v>36</v>
@@ -2426,13 +2575,13 @@
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>207</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -2450,13 +2599,13 @@
         <v>185</v>
       </c>
       <c r="AD14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AF14" t="s">
-        <v>99</v>
+        <v>218</v>
       </c>
       <c r="AJ14" t="s">
         <v>37</v>
@@ -2467,13 +2616,13 @@
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>208</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -2491,13 +2640,13 @@
         <v>91</v>
       </c>
       <c r="AD15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AE15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="AF15" t="s">
-        <v>100</v>
+        <v>219</v>
       </c>
       <c r="AJ15" t="s">
         <v>38</v>
@@ -2508,13 +2657,13 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -2532,13 +2681,13 @@
         <v>92</v>
       </c>
       <c r="AD16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AE16" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="AF16" t="s">
-        <v>101</v>
+        <v>220</v>
       </c>
       <c r="AJ16" t="s">
         <v>39</v>
@@ -2549,13 +2698,13 @@
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -2573,13 +2722,13 @@
         <v>93</v>
       </c>
       <c r="AD17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AE17" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AF17" t="s">
-        <v>102</v>
+        <v>221</v>
       </c>
       <c r="AJ17" t="s">
         <v>40</v>
@@ -2590,22 +2739,22 @@
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
       <c r="AD18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AE18" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="AF18" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
       <c r="AJ18" t="s">
         <v>42</v>
@@ -2646,6 +2795,165 @@
     <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AN23" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>192</v>
+      </c>
+      <c r="E26" t="s">
+        <v>193</v>
+      </c>
+      <c r="I26" t="s">
+        <v>199</v>
+      </c>
+      <c r="M26" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" t="s">
+        <v>192</v>
+      </c>
+      <c r="I27" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" t="s">
+        <v>192</v>
+      </c>
+      <c r="M27" t="s">
+        <v>27</v>
+      </c>
+      <c r="N27" t="s">
+        <v>28</v>
+      </c>
+      <c r="O27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" t="s">
+        <v>194</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" t="s">
+        <v>196</v>
+      </c>
+      <c r="M28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" t="s">
+        <v>29</v>
+      </c>
+      <c r="O28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" t="s">
+        <v>195</v>
+      </c>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" t="s">
+        <v>197</v>
+      </c>
+      <c r="M29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" t="s">
+        <v>198</v>
+      </c>
+      <c r="M30" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" t="s">
+        <v>45</v>
+      </c>
+      <c r="O30" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2663,7 +2971,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="9">
+  <tableParts count="13">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -2673,6 +2981,10 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>